<commit_message>
Cập nhật thống kê Lab1.
</commit_message>
<xml_diff>
--- a/Lab1/Statistic.xlsx
+++ b/Lab1/Statistic.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="G" sheetId="1" r:id="rId1"/>
-    <sheet name="GMM" sheetId="2" r:id="rId2"/>
+    <sheet name="Gauss_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Gauss_2" sheetId="3" r:id="rId2"/>
+    <sheet name="GMM_1" sheetId="2" r:id="rId3"/>
+    <sheet name="GMM_2" sheetId="4" r:id="rId4"/>
+    <sheet name="GMM_3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="42">
   <si>
     <t>SV0001_23</t>
   </si>
@@ -118,6 +121,30 @@
   <si>
     <t>Result</t>
   </si>
+  <si>
+    <t>SV0044</t>
+  </si>
+  <si>
+    <t>SV0044_30</t>
+  </si>
+  <si>
+    <t>SV0044_31</t>
+  </si>
+  <si>
+    <t>SV0044_32</t>
+  </si>
+  <si>
+    <t>SV0044_33</t>
+  </si>
+  <si>
+    <t>SV0044_34</t>
+  </si>
+  <si>
+    <t>(25,100)</t>
+  </si>
+  <si>
+    <t>(38,100)</t>
+  </si>
 </sst>
 </file>
 
@@ -205,14 +232,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -514,7 +534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -603,15 +623,15 @@
         <v>1.2226773399999999E-6</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G26" si="0">MAX(B3:F3)</f>
+        <f>MAX(B3:F3)</f>
         <v>5.160618363E-6</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f t="shared" ref="H3:H26" si="1">IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I26" si="2">IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -635,15 +655,15 @@
         <v>1.425355035E-6</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B4:F4)</f>
         <v>6.5912884370000002E-6</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -667,15 +687,15 @@
         <v>1.105947051E-6</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B5:F5)</f>
         <v>6.3166814210000003E-6</v>
       </c>
       <c r="H5" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -699,15 +719,15 @@
         <v>1.0470857770000001E-6</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B6:F6)</f>
         <v>4.3122605559999998E-6</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -731,15 +751,15 @@
         <v>1.591670319E-6</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B7:F7)</f>
         <v>6.2638365140000002E-6</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -763,15 +783,15 @@
         <v>1.6840478799999999E-6</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B8:F8)</f>
         <v>6.0921849700000002E-6</v>
       </c>
       <c r="H8" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -795,15 +815,15 @@
         <v>1.570174306E-6</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B9:F9)</f>
         <v>4.0870631040000002E-6</v>
       </c>
       <c r="H9" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -827,15 +847,15 @@
         <v>2.6906440519999998E-6</v>
       </c>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B10:F10)</f>
         <v>1.0442201094000001E-5</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -859,15 +879,15 @@
         <v>1.2664723960000001E-6</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B11:F11)</f>
         <v>4.940628829E-6</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -891,15 +911,15 @@
         <v>2.7006155310000001E-6</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B12:F12)</f>
         <v>1.1642725208E-5</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -923,15 +943,15 @@
         <v>1.7789531110000001E-6</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B13:F13)</f>
         <v>7.3901444140000002E-6</v>
       </c>
       <c r="H13" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -955,15 +975,15 @@
         <v>2.3051690939999999E-6</v>
       </c>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B14:F14)</f>
         <v>1.1360673357E-5</v>
       </c>
       <c r="H14" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -987,15 +1007,15 @@
         <v>1.8930290350000001E-6</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B15:F15)</f>
         <v>8.9101615080000004E-6</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1019,15 +1039,15 @@
         <v>1.175933084E-6</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B16:F16)</f>
         <v>6.0597666489999996E-6</v>
       </c>
       <c r="H16" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1051,15 +1071,15 @@
         <v>2.5828559169999999E-6</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B17:F17)</f>
         <v>1.3860923337000001E-5</v>
       </c>
       <c r="H17" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1083,15 +1103,15 @@
         <v>8.6544604899999997E-7</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B18:F18)</f>
         <v>4.3431757609999998E-6</v>
       </c>
       <c r="H18" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1115,15 +1135,15 @@
         <v>1.0178206689999999E-6</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B19:F19)</f>
         <v>4.7087950859999999E-6</v>
       </c>
       <c r="H19" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1147,15 +1167,15 @@
         <v>1.4580513339999999E-6</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B20:F20)</f>
         <v>8.1579945470000003E-6</v>
       </c>
       <c r="H20" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1179,15 +1199,15 @@
         <v>1.312137755E-6</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B21:F21)</f>
         <v>5.4567185550000003E-6</v>
       </c>
       <c r="H21" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -1211,15 +1231,15 @@
         <v>9.2462897999999999E-7</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B22:F22)</f>
         <v>4.5750947479999996E-6</v>
       </c>
       <c r="H22" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1243,15 +1263,15 @@
         <v>1.819343242E-6</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B23:F23)</f>
         <v>9.6599092970000006E-6</v>
       </c>
       <c r="H23" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1275,15 +1295,15 @@
         <v>1.2415650180000001E-6</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B24:F24)</f>
         <v>5.5067829469999996E-6</v>
       </c>
       <c r="H24" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1307,15 +1327,15 @@
         <v>1.1697831500000001E-6</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B25:F25)</f>
         <v>5.0075447599999996E-6</v>
       </c>
       <c r="H25" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1339,15 +1359,15 @@
         <v>7.9537516999999997E-7</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="0"/>
+        <f>MAX(B26:F26)</f>
         <v>3.771677218E-6</v>
       </c>
       <c r="H26" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -1364,6 +1384,858 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5.20993704E-7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.317674592E-6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.520021398E-6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8.9882141799999995E-7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>6.8586773900000004E-7</v>
+      </c>
+      <c r="G2" s="2">
+        <f>MAX(B2:F2)</f>
+        <v>2.317674592E-6</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5.3705824000000004E-7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.818225903E-6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.271859457E-6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.2226773399999999E-6</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7.0745002099999997E-7</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G26" si="0">MAX(B3:F3)</f>
+        <v>2.818225903E-6</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f t="shared" ref="H3:H26" si="1">IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I26" si="2">IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>6.2440351899999996E-7</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.4527516749999999E-6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.224532487E-6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.425355035E-6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0139227770000001E-6</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4527516749999999E-6</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4.2380916300000002E-7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.0255080329999999E-6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.827424572E-6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.105947051E-6</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8.0934033800000003E-7</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0255080329999999E-6</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>6.1058576200000005E-7</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.6363089739999998E-6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.2553281599999999E-6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.0470857770000001E-6</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.0703280699999996E-7</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6363089739999998E-6</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>5.9714873800000005E-7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.735101752E-6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.2728856879999998E-6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.591670319E-6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.086708637E-6</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>3.735101752E-6</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6.3735754799999998E-7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4.103172021E-6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.3028198149999999E-6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.6840478799999999E-6</v>
+      </c>
+      <c r="F8" s="2">
+        <v>8.9207726900000002E-7</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.103172021E-6</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.5377105700000003E-7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.5234272509999999E-6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.540826971E-6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.570174306E-6</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7.3398813000000002E-7</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>3.5234272509999999E-6</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8.0719250299999999E-7</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.5773115950000004E-6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5.6673784839999996E-6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.6906440519999998E-6</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.3381887370000001E-6</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5773115950000004E-6</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>4.48034927E-7</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.158190856E-6</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2.500722677E-6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.2664723960000001E-6</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7.2227898399999995E-7</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>3.158190856E-6</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7.5180735799999995E-7</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.3577356689999998E-6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6.0711887269999999E-6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2.7006155310000001E-6</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.329166748E-6</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>6.3577356689999998E-6</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>6.1383249299999998E-7</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4.2663389980000004E-6</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4.2795891009999998E-6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.7789531110000001E-6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>9.4687763799999997E-7</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>4.2795891009999998E-6</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0007</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>8.1533340299999999E-7</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.2774703309999997E-6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.6315635049999996E-6</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.3051690939999999E-6</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.2433458829999999E-6</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.2774703309999997E-6</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>5.2413650899999997E-7</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.6835971299999999E-6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4.7937708659999997E-6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.8930290350000001E-6</v>
+      </c>
+      <c r="F15" s="2">
+        <v>9.0018870399999997E-7</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>4.7937708659999997E-6</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0007</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.4902474000000002E-7</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.1521503909999998E-6</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.827124185E-6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.175933084E-6</v>
+      </c>
+      <c r="F16" s="2">
+        <v>7.6688617699999996E-7</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1521503909999998E-6</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.7278792499999999E-7</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.3935453679999999E-6</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2.2203148410000001E-6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9.2462897999999999E-7</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5.1286136000000001E-7</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="0"/>
+        <v>2.3935453679999999E-6</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>5.86241623E-7</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4.6879013999999996E-6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4.8233903909999998E-6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.819343242E-6</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.4292478700000003E-7</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>4.8233903909999998E-6</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0007</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.4674266799999998E-7</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.9558071799999999E-6</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2.7488864699999999E-6</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.2415650180000001E-6</v>
+      </c>
+      <c r="F19" s="2">
+        <v>6.47694088E-7</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9558071799999999E-6</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.2592972400000001E-7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.6160260480000001E-6</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2.5914885289999999E-6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.1697831500000001E-6</v>
+      </c>
+      <c r="F20" s="2">
+        <v>7.4582485799999998E-7</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>2.6160260480000001E-6</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.7398788199999997E-7</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2.048847642E-6</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.8992288660000001E-6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7.9537516999999997E-7</v>
+      </c>
+      <c r="F21" s="2">
+        <v>4.7560608099999998E-7</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>2.048847642E-6</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2.31551036E-7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6.7487360000000004E-7</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5.8177783799999995E-7</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.1062348800000001E-7</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5.75218354E-7</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>6.7487360000000004E-7</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.5199346299999999E-7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4.6054825800000001E-7</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.7276984399999999E-7</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2.9651082599999998E-7</v>
+      </c>
+      <c r="F23" s="2">
+        <v>4.1631025100000001E-7</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6054825800000001E-7</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.4541495899999999E-7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5.7633258900000005E-7</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4.25389921E-7</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.93347253E-7</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3.5096214700000002E-7</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>5.7633258900000005E-7</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.93582133E-7</v>
+      </c>
+      <c r="C25" s="2">
+        <v>9.5963885600000001E-7</v>
+      </c>
+      <c r="D25" s="2">
+        <v>8.1373246699999997E-7</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5.1846008400000004E-7</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5.55280705E-7</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>9.5963885600000001E-7</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2.03644615E-7</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.1132746550000001E-6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6.9993692099999995E-7</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.69130054E-7</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3.9855537299999999E-7</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1132746550000001E-6</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>SV0002</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="7">
+        <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
@@ -2217,4 +3089,1520 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4.1875692120999999E-5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.34652364242E-4</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3.8775334597000003E-5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.6455927821999998E-5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>3.1868502402000001E-5</v>
+      </c>
+      <c r="G2" s="2">
+        <f>MAX(B2:F2)</f>
+        <v>1.34652364242E-4</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.43097998738E-4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.059547511698E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.0285020010399999E-4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9.0146493867000003E-5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.08298916263E-4</v>
+      </c>
+      <c r="G3" s="2">
+        <f>MAX(B3:F3)</f>
+        <v>1.059547511698E-3</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.179238465888E-3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4.1124369873842E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.7078587600385E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.3994512606092E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.6999623465160001E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <f>MAX(B4:F4)</f>
+        <v>4.1124369873842E-2</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.2293963574588999E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>7.4643306718959099</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9.0516455796675093</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12.5890430062438</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.37782690415173897</v>
+      </c>
+      <c r="G5" s="2">
+        <f>MAX(B5:F5)</f>
+        <v>12.5890430062438</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
+        <v>SV0041</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4.4131200981999999E-5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.47253323158E-4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.20573057798E-4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.75941137867E-4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8.6245107551000005E-5</v>
+      </c>
+      <c r="G6" s="2">
+        <f>MAX(B6:F6)</f>
+        <v>3.20573057798E-4</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2.5192134302439999E-3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.2153918788436102</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.74137339511483</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.85304187381291</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6.4248932174417003E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <f>MAX(B7:F7)</f>
+        <v>2.2153918788436102</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.8023378636449999E-3</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.12147825278839</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2.9086503913899999E-3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>8.7479164763550003E-3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>3.784744982566E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <f>MAX(B8:F8)</f>
+        <v>0.12147825278839</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.1878882016E-4</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5.7839721537980997E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4.6517433238200002E-4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.1466140490680001E-3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.229707380309E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <f>MAX(B9:F9)</f>
+        <v>5.7839721537980997E-2</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5.8243729244289999E-3</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.43887278278261699</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.49909923121101102</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.4023018077541998E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7.4170258546119999E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f>MAX(B10:F10)</f>
+        <v>0.49909923121101102</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6.0134213227540003E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.87516178074344197</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.100397065705684</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.9349115616674999E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4.5632861429181E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f>MAX(B11:F11)</f>
+        <v>0.87516178074344197</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2">
+        <v>9.3779928229199994E-3</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.3230485492821504</v>
+      </c>
+      <c r="D12" s="2">
+        <v>113.91824129403901</v>
+      </c>
+      <c r="E12" s="2">
+        <v>168.305396675683</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.863819364342573</v>
+      </c>
+      <c r="G12" s="2">
+        <f>MAX(B12:F12)</f>
+        <v>168.305396675683</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
+        <v>SV0041</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4.2994624334179998E-3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.18246510194266</v>
+      </c>
+      <c r="D13" s="2">
+        <v>22.8418781647432</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.5343672430434701</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0.99263767448576301</v>
+      </c>
+      <c r="G13" s="2">
+        <f>MAX(B13:F13)</f>
+        <v>22.8418781647432</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6.9562854429900001E-3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.8417665277452802</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5.1484419703585296</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3.6633190187964702</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.14869267754252199</v>
+      </c>
+      <c r="G14" s="2">
+        <f>MAX(B14:F14)</f>
+        <v>5.1484419703585296</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7.1494827199520003E-3</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.1236900400814296</v>
+      </c>
+      <c r="D15" s="2">
+        <v>614.95783532235203</v>
+      </c>
+      <c r="E15" s="2">
+        <v>331.39547365645598</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1.2113728053345001</v>
+      </c>
+      <c r="G15" s="2">
+        <f>MAX(B15:F15)</f>
+        <v>614.95783532235203</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2">
+        <v>7.3746214345489997E-3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4.1634450933430402</v>
+      </c>
+      <c r="D16" s="2">
+        <v>22.661452030299898</v>
+      </c>
+      <c r="E16" s="2">
+        <v>3.57344799390123</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.35360109215416602</v>
+      </c>
+      <c r="G16" s="2">
+        <f>MAX(B16:F16)</f>
+        <v>22.661452030299898</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>4.0364810668000002E-3</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4.04266902543299</v>
+      </c>
+      <c r="D17" s="2">
+        <v>91.288633237467707</v>
+      </c>
+      <c r="E17" s="2">
+        <v>180.79571005950601</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1.00478126952839</v>
+      </c>
+      <c r="G17" s="2">
+        <f>MAX(B17:F17)</f>
+        <v>180.79571005950601</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
+        <v>SV0041</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2.2474207658129998E-3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2.4380313387507302</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1840.7176988423701</v>
+      </c>
+      <c r="E18" s="2">
+        <v>46560.5900277658</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.9737188409484001</v>
+      </c>
+      <c r="G18" s="2">
+        <f>MAX(B18:F18)</f>
+        <v>46560.5900277658</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
+        <v>SV0041</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5.1447603974699996E-3</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.56764607142531</v>
+      </c>
+      <c r="D19" s="2">
+        <v>51.3003635920861</v>
+      </c>
+      <c r="E19" s="2">
+        <v>17.5208466157505</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.32343040107967602</v>
+      </c>
+      <c r="G19" s="2">
+        <f>MAX(B19:F19)</f>
+        <v>51.3003635920861</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.2027749897260002E-3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.2558638268846698</v>
+      </c>
+      <c r="D20" s="2">
+        <v>130.81309976640301</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1626.7889864947001</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.27712953977946497</v>
+      </c>
+      <c r="G20" s="2">
+        <f>MAX(B20:F20)</f>
+        <v>1626.7889864947001</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
+        <v>SV0041</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.3430948519810001E-3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.27145285688584803</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4.1952614539950001E-2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>8.0329680558510006E-3</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1.0537654961971E-2</v>
+      </c>
+      <c r="G21" s="2">
+        <f>MAX(B21:F21)</f>
+        <v>0.27145285688584803</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2">
+        <v>4.4712238799999998E-7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.6256870339999999E-6</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.3026496429450001E-3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.1844344166799998E-4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.0700632831299999E-4</v>
+      </c>
+      <c r="G22" s="2">
+        <f>MAX(B22:F22)</f>
+        <v>3.3026496429450001E-3</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2.9077729900000001E-7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.687767312E-6</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6.5404608780000001E-6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>8.0733784899999995E-7</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2.3141849456000001E-5</v>
+      </c>
+      <c r="G23" s="2">
+        <f>MAX(B23:F23)</f>
+        <v>2.3141849456000001E-5</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
+        <v>SV0044</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2">
+        <v>9.5372061717999995E-5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>7.879318263E-6</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.7857103249999999E-6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.114250656E-6</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.6430287817E-5</v>
+      </c>
+      <c r="G24" s="2">
+        <f>MAX(B24:F24)</f>
+        <v>9.5372061717999995E-5</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2">
+        <v>8.9347272179800003E-4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>6.4164478208277004E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.4728892546029999E-3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2.4748095038909998E-3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>3.6151556306640999E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f>MAX(B25:F25)</f>
+        <v>6.4164478208277004E-2</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.3400424963200001E-4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.02900827827E-4</v>
+      </c>
+      <c r="D26" s="2">
+        <v>7.4006982009000005E-5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>6.8290283139999997E-5</v>
+      </c>
+      <c r="F26" s="2">
+        <v>2.988694298513E-3</v>
+      </c>
+      <c r="G26" s="2">
+        <f>MAX(B26:F26)</f>
+        <v>2.988694298513E-3</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
+        <v>SV0044</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="7">
+        <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
+        <v>0.52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <f>MAX(B2:F2)</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <f>MAX(B3:F3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <f>MAX(B4:F4)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <f>MAX(B5:F5)</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <f>MAX(B6:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <f>MAX(B7:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <f>MAX(B8:F8)</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <f>MAX(B9:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <f>MAX(B10:F10)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <f>MAX(B11:F11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="str">
+        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <f>MAX(B12:F12)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="str">
+        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <f>MAX(B13:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="str">
+        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <f>MAX(B14:F14)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="str">
+        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
+        <f>MAX(B15:F15)</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <f>MAX(B16:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="str">
+        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <f>MAX(B17:F17)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="str">
+        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <f>MAX(B18:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2" t="str">
+        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <f>MAX(B19:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="str">
+        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2">
+        <f>MAX(B20:F20)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="str">
+        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
+        <f>MAX(B21:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="str">
+        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3.43365188E-7</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.468321426E-6</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2.4869391059069998E-3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>8.1619302808999994E-5</v>
+      </c>
+      <c r="F22" s="2">
+        <v>8.9976757852999994E-5</v>
+      </c>
+      <c r="G22" s="2">
+        <f>MAX(B22:F22)</f>
+        <v>2.4869391059069998E-3</v>
+      </c>
+      <c r="H22" s="2" t="str">
+        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
+        <v>SV0007</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.1233670800000002E-7</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.100811068E-6</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6.2640250230000003E-6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3.2215572520000001E-6</v>
+      </c>
+      <c r="F23" s="2">
+        <v>6.4386189484E-5</v>
+      </c>
+      <c r="G23" s="2">
+        <f>MAX(B23:F23)</f>
+        <v>6.4386189484E-5</v>
+      </c>
+      <c r="H23" s="2" t="str">
+        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
+        <v>SV0044</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2">
+        <v>9.4832263917000005E-5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>5.3023832559999997E-6</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.880532427E-6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.0470341900000002E-6</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3.2852448390999999E-5</v>
+      </c>
+      <c r="G24" s="2">
+        <f>MAX(B24:F24)</f>
+        <v>9.4832263917000005E-5</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
+        <v>SV0001</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7.9485853244999996E-4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.12783303428942799</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9.2142152476160002E-3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2.2619171550639998E-3</v>
+      </c>
+      <c r="F25" s="2">
+        <v>8.4026184479928004E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f>MAX(B25:F25)</f>
+        <v>0.12783303428942799</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
+        <v>SV0002</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.6935860305299999E-4</v>
+      </c>
+      <c r="C26" s="2">
+        <v>4.8501551259999998E-5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.01855893874E-4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.6114369497799999E-4</v>
+      </c>
+      <c r="F26" s="2">
+        <v>4.2195553201679996E-3</v>
+      </c>
+      <c r="G26" s="2">
+        <f>MAX(B26:F26)</f>
+        <v>4.2195553201679996E-3</v>
+      </c>
+      <c r="H26" s="2" t="str">
+        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
+        <v>SV0044</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="7">
+        <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Bổ sung báo cáo Lab1.
</commit_message>
<xml_diff>
--- a/Lab1/Statistic.xlsx
+++ b/Lab1/Statistic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Gauss_1" sheetId="1" r:id="rId1"/>
@@ -150,8 +150,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000000000000"/>
+    <numFmt numFmtId="180" formatCode="#,##0.0000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -216,7 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -227,6 +229,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -591,15 +603,15 @@
         <v>8.9882141844466398E-7</v>
       </c>
       <c r="G2" s="2">
-        <f>MAX(B2:F2)</f>
+        <f t="shared" ref="G2:G26" si="0">MAX(B2:F2)</f>
         <v>3.6596353751972801E-6</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <f t="shared" ref="H2:H26" si="1">IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
         <v>SV0040</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <f t="shared" ref="I2:I26" si="2">IF(LEFT(A2,6)=H2, "Yes", "")</f>
         <v/>
       </c>
     </row>
@@ -623,15 +635,15 @@
         <v>1.2226773399999999E-6</v>
       </c>
       <c r="G3" s="2">
-        <f>MAX(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>5.160618363E-6</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -655,15 +667,15 @@
         <v>1.425355035E-6</v>
       </c>
       <c r="G4" s="2">
-        <f>MAX(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>6.5912884370000002E-6</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -687,15 +699,15 @@
         <v>1.105947051E-6</v>
       </c>
       <c r="G5" s="2">
-        <f>MAX(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>6.3166814210000003E-6</v>
       </c>
       <c r="H5" s="2" t="str">
-        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -719,15 +731,15 @@
         <v>1.0470857770000001E-6</v>
       </c>
       <c r="G6" s="2">
-        <f>MAX(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>4.3122605559999998E-6</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -751,15 +763,15 @@
         <v>1.591670319E-6</v>
       </c>
       <c r="G7" s="2">
-        <f>MAX(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>6.2638365140000002E-6</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -783,15 +795,15 @@
         <v>1.6840478799999999E-6</v>
       </c>
       <c r="G8" s="2">
-        <f>MAX(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>6.0921849700000002E-6</v>
       </c>
       <c r="H8" s="2" t="str">
-        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -815,15 +827,15 @@
         <v>1.570174306E-6</v>
       </c>
       <c r="G9" s="2">
-        <f>MAX(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>4.0870631040000002E-6</v>
       </c>
       <c r="H9" s="2" t="str">
-        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -847,15 +859,15 @@
         <v>2.6906440519999998E-6</v>
       </c>
       <c r="G10" s="2">
-        <f>MAX(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>1.0442201094000001E-5</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -879,15 +891,15 @@
         <v>1.2664723960000001E-6</v>
       </c>
       <c r="G11" s="2">
-        <f>MAX(B11:F11)</f>
+        <f t="shared" si="0"/>
         <v>4.940628829E-6</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -911,15 +923,15 @@
         <v>2.7006155310000001E-6</v>
       </c>
       <c r="G12" s="2">
-        <f>MAX(B12:F12)</f>
+        <f t="shared" si="0"/>
         <v>1.1642725208E-5</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -943,15 +955,15 @@
         <v>1.7789531110000001E-6</v>
       </c>
       <c r="G13" s="2">
-        <f>MAX(B13:F13)</f>
+        <f t="shared" si="0"/>
         <v>7.3901444140000002E-6</v>
       </c>
       <c r="H13" s="2" t="str">
-        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -975,15 +987,15 @@
         <v>2.3051690939999999E-6</v>
       </c>
       <c r="G14" s="2">
-        <f>MAX(B14:F14)</f>
+        <f t="shared" si="0"/>
         <v>1.1360673357E-5</v>
       </c>
       <c r="H14" s="2" t="str">
-        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1007,15 +1019,15 @@
         <v>1.8930290350000001E-6</v>
       </c>
       <c r="G15" s="2">
-        <f>MAX(B15:F15)</f>
+        <f t="shared" si="0"/>
         <v>8.9101615080000004E-6</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1039,15 +1051,15 @@
         <v>1.175933084E-6</v>
       </c>
       <c r="G16" s="2">
-        <f>MAX(B16:F16)</f>
+        <f t="shared" si="0"/>
         <v>6.0597666489999996E-6</v>
       </c>
       <c r="H16" s="2" t="str">
-        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1071,15 +1083,15 @@
         <v>2.5828559169999999E-6</v>
       </c>
       <c r="G17" s="2">
-        <f>MAX(B17:F17)</f>
+        <f t="shared" si="0"/>
         <v>1.3860923337000001E-5</v>
       </c>
       <c r="H17" s="2" t="str">
-        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -1103,15 +1115,15 @@
         <v>8.6544604899999997E-7</v>
       </c>
       <c r="G18" s="2">
-        <f>MAX(B18:F18)</f>
+        <f t="shared" si="0"/>
         <v>4.3431757609999998E-6</v>
       </c>
       <c r="H18" s="2" t="str">
-        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -1135,15 +1147,15 @@
         <v>1.0178206689999999E-6</v>
       </c>
       <c r="G19" s="2">
-        <f>MAX(B19:F19)</f>
+        <f t="shared" si="0"/>
         <v>4.7087950859999999E-6</v>
       </c>
       <c r="H19" s="2" t="str">
-        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -1167,15 +1179,15 @@
         <v>1.4580513339999999E-6</v>
       </c>
       <c r="G20" s="2">
-        <f>MAX(B20:F20)</f>
+        <f t="shared" si="0"/>
         <v>8.1579945470000003E-6</v>
       </c>
       <c r="H20" s="2" t="str">
-        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -1199,15 +1211,15 @@
         <v>1.312137755E-6</v>
       </c>
       <c r="G21" s="2">
-        <f>MAX(B21:F21)</f>
+        <f t="shared" si="0"/>
         <v>5.4567185550000003E-6</v>
       </c>
       <c r="H21" s="2" t="str">
-        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -1231,15 +1243,15 @@
         <v>9.2462897999999999E-7</v>
       </c>
       <c r="G22" s="2">
-        <f>MAX(B22:F22)</f>
+        <f t="shared" si="0"/>
         <v>4.5750947479999996E-6</v>
       </c>
       <c r="H22" s="2" t="str">
-        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1263,15 +1275,15 @@
         <v>1.819343242E-6</v>
       </c>
       <c r="G23" s="2">
-        <f>MAX(B23:F23)</f>
+        <f t="shared" si="0"/>
         <v>9.6599092970000006E-6</v>
       </c>
       <c r="H23" s="2" t="str">
-        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1295,15 +1307,15 @@
         <v>1.2415650180000001E-6</v>
       </c>
       <c r="G24" s="2">
-        <f>MAX(B24:F24)</f>
+        <f t="shared" si="0"/>
         <v>5.5067829469999996E-6</v>
       </c>
       <c r="H24" s="2" t="str">
-        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1327,15 +1339,15 @@
         <v>1.1697831500000001E-6</v>
       </c>
       <c r="G25" s="2">
-        <f>MAX(B25:F25)</f>
+        <f t="shared" si="0"/>
         <v>5.0075447599999996E-6</v>
       </c>
       <c r="H25" s="2" t="str">
-        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1359,15 +1371,15 @@
         <v>7.9537516999999997E-7</v>
       </c>
       <c r="G26" s="2">
-        <f>MAX(B26:F26)</f>
+        <f t="shared" si="0"/>
         <v>3.771677218E-6</v>
       </c>
       <c r="H26" s="2" t="str">
-        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0040</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -1387,7 +1399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1428,19 +1442,19 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>5.20993704E-7</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="8">
         <v>2.317674592E-6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="8">
         <v>1.520021398E-6</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="8">
         <v>8.9882141799999995E-7</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="8">
         <v>6.8586773900000004E-7</v>
       </c>
       <c r="G2" s="2">
@@ -1460,19 +1474,19 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="9">
         <v>5.3705824000000004E-7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="8">
         <v>2.818225903E-6</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="8">
         <v>2.271859457E-6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>1.2226773399999999E-6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="8">
         <v>7.0745002099999997E-7</v>
       </c>
       <c r="G3" s="2">
@@ -1492,19 +1506,19 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="9">
         <v>6.2440351899999996E-7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="8">
         <v>3.4527516749999999E-6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="8">
         <v>3.224532487E-6</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>1.425355035E-6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="8">
         <v>1.0139227770000001E-6</v>
       </c>
       <c r="G4" s="2">
@@ -1524,19 +1538,19 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="9">
         <v>4.2380916300000002E-7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="8">
         <v>3.0255080329999999E-6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>2.827424572E-6</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="8">
         <v>1.105947051E-6</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="8">
         <v>8.0934033800000003E-7</v>
       </c>
       <c r="G5" s="2">
@@ -1556,19 +1570,19 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="9">
         <v>6.1058576200000005E-7</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="8">
         <v>2.6363089739999998E-6</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="8">
         <v>2.2553281599999999E-6</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>1.0470857770000001E-6</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="8">
         <v>8.0703280699999996E-7</v>
       </c>
       <c r="G6" s="2">
@@ -1588,19 +1602,19 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="8">
         <v>5.9714873800000005E-7</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="8">
         <v>3.735101752E-6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="8">
         <v>3.2728856879999998E-6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="8">
         <v>1.591670319E-6</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="8">
         <v>1.086708637E-6</v>
       </c>
       <c r="G7" s="2">
@@ -1620,19 +1634,19 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="8">
         <v>6.3735754799999998E-7</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="8">
         <v>4.103172021E-6</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="8">
         <v>3.3028198149999999E-6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>1.6840478799999999E-6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="8">
         <v>8.9207726900000002E-7</v>
       </c>
       <c r="G8" s="2">
@@ -1652,19 +1666,19 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="8">
         <v>6.5377105700000003E-7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="8">
         <v>3.5234272509999999E-6</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="8">
         <v>2.540826971E-6</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>1.570174306E-6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="8">
         <v>7.3398813000000002E-7</v>
       </c>
       <c r="G9" s="2">
@@ -1684,19 +1698,19 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="8">
         <v>8.0719250299999999E-7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="8">
         <v>6.5773115950000004E-6</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="8">
         <v>5.6673784839999996E-6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="8">
         <v>2.6906440519999998E-6</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="8">
         <v>1.3381887370000001E-6</v>
       </c>
       <c r="G10" s="2">
@@ -1716,19 +1730,19 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="8">
         <v>4.48034927E-7</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="8">
         <v>3.158190856E-6</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="8">
         <v>2.500722677E-6</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="8">
         <v>1.2664723960000001E-6</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="8">
         <v>7.2227898399999995E-7</v>
       </c>
       <c r="G11" s="2">
@@ -1748,19 +1762,19 @@
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="8">
         <v>7.5180735799999995E-7</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="8">
         <v>6.3577356689999998E-6</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="8">
         <v>6.0711887269999999E-6</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="8">
         <v>2.7006155310000001E-6</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="8">
         <v>1.329166748E-6</v>
       </c>
       <c r="G12" s="2">
@@ -1780,19 +1794,19 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="8">
         <v>6.1383249299999998E-7</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="8">
         <v>4.2663389980000004E-6</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="8">
         <v>4.2795891009999998E-6</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>1.7789531110000001E-6</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="8">
         <v>9.4687763799999997E-7</v>
       </c>
       <c r="G13" s="2">
@@ -1812,19 +1826,19 @@
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="8">
         <v>8.1533340299999999E-7</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="8">
         <v>6.2774703309999997E-6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="8">
         <v>5.6315635049999996E-6</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="8">
         <v>2.3051690939999999E-6</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="8">
         <v>1.2433458829999999E-6</v>
       </c>
       <c r="G14" s="2">
@@ -1844,19 +1858,19 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="8">
         <v>5.2413650899999997E-7</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="8">
         <v>4.6835971299999999E-6</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="8">
         <v>4.7937708659999997E-6</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="8">
         <v>1.8930290350000001E-6</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="8">
         <v>9.0018870399999997E-7</v>
       </c>
       <c r="G15" s="2">
@@ -1876,19 +1890,19 @@
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="8">
         <v>4.4902474000000002E-7</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="8">
         <v>3.1521503909999998E-6</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="8">
         <v>2.827124185E-6</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="8">
         <v>1.175933084E-6</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="8">
         <v>7.6688617699999996E-7</v>
       </c>
       <c r="G16" s="2">
@@ -1908,19 +1922,19 @@
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="8">
         <v>2.7278792499999999E-7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="8">
         <v>2.3935453679999999E-6</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="8">
         <v>2.2203148410000001E-6</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="8">
         <v>9.2462897999999999E-7</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="8">
         <v>5.1286136000000001E-7</v>
       </c>
       <c r="G17" s="2">
@@ -1940,19 +1954,19 @@
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="8">
         <v>5.86241623E-7</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="8">
         <v>4.6879013999999996E-6</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="8">
         <v>4.8233903909999998E-6</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="8">
         <v>1.819343242E-6</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="8">
         <v>9.4292478700000003E-7</v>
       </c>
       <c r="G18" s="2">
@@ -1972,19 +1986,19 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="8">
         <v>3.4674266799999998E-7</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="8">
         <v>2.9558071799999999E-6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="8">
         <v>2.7488864699999999E-6</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="8">
         <v>1.2415650180000001E-6</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="8">
         <v>6.47694088E-7</v>
       </c>
       <c r="G19" s="2">
@@ -2004,19 +2018,19 @@
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="8">
         <v>3.2592972400000001E-7</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="8">
         <v>2.6160260480000001E-6</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="8">
         <v>2.5914885289999999E-6</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="8">
         <v>1.1697831500000001E-6</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="8">
         <v>7.4582485799999998E-7</v>
       </c>
       <c r="G20" s="2">
@@ -2036,19 +2050,19 @@
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="8">
         <v>2.7398788199999997E-7</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="8">
         <v>2.048847642E-6</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="8">
         <v>1.8992288660000001E-6</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="8">
         <v>7.9537516999999997E-7</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="8">
         <v>4.7560608099999998E-7</v>
       </c>
       <c r="G21" s="2">
@@ -2068,19 +2082,19 @@
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="8">
         <v>2.31551036E-7</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="8">
         <v>6.7487360000000004E-7</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="8">
         <v>5.8177783799999995E-7</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="8">
         <v>4.1062348800000001E-7</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="8">
         <v>5.75218354E-7</v>
       </c>
       <c r="G22" s="2">
@@ -2100,19 +2114,19 @@
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="8">
         <v>1.5199346299999999E-7</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="8">
         <v>4.6054825800000001E-7</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="8">
         <v>3.7276984399999999E-7</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="8">
         <v>2.9651082599999998E-7</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="8">
         <v>4.1631025100000001E-7</v>
       </c>
       <c r="G23" s="2">
@@ -2132,19 +2146,19 @@
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="8">
         <v>1.4541495899999999E-7</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="8">
         <v>5.7633258900000005E-7</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="8">
         <v>4.25389921E-7</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="8">
         <v>2.93347253E-7</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="8">
         <v>3.5096214700000002E-7</v>
       </c>
       <c r="G24" s="2">
@@ -2164,19 +2178,19 @@
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="8">
         <v>1.93582133E-7</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="8">
         <v>9.5963885600000001E-7</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="8">
         <v>8.1373246699999997E-7</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="8">
         <v>5.1846008400000004E-7</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="8">
         <v>5.55280705E-7</v>
       </c>
       <c r="G25" s="2">
@@ -2196,19 +2210,19 @@
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="8">
         <v>2.03644615E-7</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="8">
         <v>1.1132746550000001E-6</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="8">
         <v>6.9993692099999995E-7</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="8">
         <v>4.69130054E-7</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="8">
         <v>3.9855537299999999E-7</v>
       </c>
       <c r="G26" s="2">
@@ -3095,37 +3109,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3139,807 +3153,807 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="11">
         <v>4.1875692120999999E-5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="11">
         <v>1.34652364242E-4</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="11">
         <v>3.8775334597000003E-5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="11">
         <v>3.6455927821999998E-5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="11">
         <v>3.1868502402000001E-5</v>
       </c>
       <c r="G2" s="2">
-        <f>MAX(B2:F2)</f>
+        <f t="shared" ref="G2:G26" si="0">MAX(B2:F2)</f>
         <v>1.34652364242E-4</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <f t="shared" ref="H2:H26" si="1">IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
         <v>SV0002</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <f t="shared" ref="I2:I26" si="2">IF(LEFT(A2,6)=H2, "Yes", "")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="12">
         <v>2.43097998738E-4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="11">
         <v>1.059547511698E-3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="11">
         <v>2.0285020010399999E-4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="11">
         <v>9.0146493867000003E-5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="11">
         <v>1.08298916263E-4</v>
       </c>
       <c r="G3" s="2">
-        <f>MAX(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>1.059547511698E-3</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="12">
         <v>1.179238465888E-3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="11">
         <v>4.1124369873842E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="11">
         <v>2.7078587600385E-2</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="11">
         <v>1.3994512606092E-2</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="11">
         <v>1.6999623465160001E-3</v>
       </c>
       <c r="G4" s="2">
-        <f>MAX(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>4.1124369873842E-2</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="12">
         <v>1.2293963574588999E-2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="11">
         <v>7.4643306718959099</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="11">
         <v>9.0516455796675093</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="11">
         <v>12.5890430062438</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="11">
         <v>0.37782690415173897</v>
       </c>
       <c r="G5" s="2">
-        <f>MAX(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>12.5890430062438</v>
       </c>
       <c r="H5" s="2" t="str">
-        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0041</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="11">
         <v>4.4131200981999999E-5</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="11">
         <v>1.47253323158E-4</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="11">
         <v>3.20573057798E-4</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="11">
         <v>1.75941137867E-4</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="11">
         <v>8.6245107551000005E-5</v>
       </c>
       <c r="G6" s="2">
-        <f>MAX(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>3.20573057798E-4</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="11">
         <v>2.5192134302439999E-3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="11">
         <v>2.2153918788436102</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="11">
         <v>1.74137339511483</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="11">
         <v>1.85304187381291</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="11">
         <v>6.4248932174417003E-2</v>
       </c>
       <c r="G7" s="2">
-        <f>MAX(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>2.2153918788436102</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="11">
         <v>1.8023378636449999E-3</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="11">
         <v>0.12147825278839</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="11">
         <v>2.9086503913899999E-3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="11">
         <v>8.7479164763550003E-3</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="11">
         <v>3.784744982566E-3</v>
       </c>
       <c r="G8" s="2">
-        <f>MAX(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>0.12147825278839</v>
       </c>
       <c r="H8" s="2" t="str">
-        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="11">
         <v>3.1878882016E-4</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="11">
         <v>5.7839721537980997E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="11">
         <v>4.6517433238200002E-4</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="11">
         <v>1.1466140490680001E-3</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="11">
         <v>1.229707380309E-3</v>
       </c>
       <c r="G9" s="2">
-        <f>MAX(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>5.7839721537980997E-2</v>
       </c>
       <c r="H9" s="2" t="str">
-        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="11">
         <v>5.8243729244289999E-3</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="11">
         <v>0.43887278278261699</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="11">
         <v>0.49909923121101102</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="11">
         <v>4.4023018077541998E-2</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="11">
         <v>7.4170258546119999E-2</v>
       </c>
       <c r="G10" s="2">
-        <f>MAX(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>0.49909923121101102</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="11">
         <v>6.0134213227540003E-3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="11">
         <v>0.87516178074344197</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="11">
         <v>0.100397065705684</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="11">
         <v>1.9349115616674999E-2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="11">
         <v>4.5632861429181E-2</v>
       </c>
       <c r="G11" s="2">
-        <f>MAX(B11:F11)</f>
+        <f t="shared" si="0"/>
         <v>0.87516178074344197</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="11">
         <v>9.3779928229199994E-3</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="11">
         <v>6.3230485492821504</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="11">
         <v>113.91824129403901</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="11">
         <v>168.305396675683</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="11">
         <v>0.863819364342573</v>
       </c>
       <c r="G12" s="2">
-        <f>MAX(B12:F12)</f>
+        <f t="shared" si="0"/>
         <v>168.305396675683</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0041</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="11">
         <v>4.2994624334179998E-3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="11">
         <v>1.18246510194266</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="11">
         <v>22.8418781647432</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="11">
         <v>1.5343672430434701</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="11">
         <v>0.99263767448576301</v>
       </c>
       <c r="G13" s="2">
-        <f>MAX(B13:F13)</f>
+        <f t="shared" si="0"/>
         <v>22.8418781647432</v>
       </c>
       <c r="H13" s="2" t="str">
-        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="11">
         <v>6.9562854429900001E-3</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="11">
         <v>2.8417665277452802</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="11">
         <v>5.1484419703585296</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="11">
         <v>3.6633190187964702</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="11">
         <v>0.14869267754252199</v>
       </c>
       <c r="G14" s="2">
-        <f>MAX(B14:F14)</f>
+        <f t="shared" si="0"/>
         <v>5.1484419703585296</v>
       </c>
       <c r="H14" s="2" t="str">
-        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="11">
         <v>7.1494827199520003E-3</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="11">
         <v>9.1236900400814296</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="11">
         <v>614.95783532235203</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="11">
         <v>331.39547365645598</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="11">
         <v>1.2113728053345001</v>
       </c>
       <c r="G15" s="2">
-        <f>MAX(B15:F15)</f>
+        <f t="shared" si="0"/>
         <v>614.95783532235203</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="11">
         <v>7.3746214345489997E-3</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="11">
         <v>4.1634450933430402</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="11">
         <v>22.661452030299898</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="11">
         <v>3.57344799390123</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="11">
         <v>0.35360109215416602</v>
       </c>
       <c r="G16" s="2">
-        <f>MAX(B16:F16)</f>
+        <f t="shared" si="0"/>
         <v>22.661452030299898</v>
       </c>
       <c r="H16" s="2" t="str">
-        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="11">
         <v>4.0364810668000002E-3</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="11">
         <v>4.04266902543299</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="11">
         <v>91.288633237467707</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="11">
         <v>180.79571005950601</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="11">
         <v>1.00478126952839</v>
       </c>
       <c r="G17" s="2">
-        <f>MAX(B17:F17)</f>
+        <f t="shared" si="0"/>
         <v>180.79571005950601</v>
       </c>
       <c r="H17" s="2" t="str">
-        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0041</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="11">
         <v>2.2474207658129998E-3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="11">
         <v>2.4380313387507302</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="11">
         <v>1840.7176988423701</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="11">
         <v>46560.5900277658</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="11">
         <v>2.9737188409484001</v>
       </c>
       <c r="G18" s="2">
-        <f>MAX(B18:F18)</f>
+        <f t="shared" si="0"/>
         <v>46560.5900277658</v>
       </c>
       <c r="H18" s="2" t="str">
-        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0041</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="11">
         <v>5.1447603974699996E-3</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="11">
         <v>3.56764607142531</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="11">
         <v>51.3003635920861</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="11">
         <v>17.5208466157505</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="11">
         <v>0.32343040107967602</v>
       </c>
       <c r="G19" s="2">
-        <f>MAX(B19:F19)</f>
+        <f t="shared" si="0"/>
         <v>51.3003635920861</v>
       </c>
       <c r="H19" s="2" t="str">
-        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="11">
         <v>3.2027749897260002E-3</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="11">
         <v>2.2558638268846698</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="11">
         <v>130.81309976640301</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="11">
         <v>1626.7889864947001</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="11">
         <v>0.27712953977946497</v>
       </c>
       <c r="G20" s="2">
-        <f>MAX(B20:F20)</f>
+        <f t="shared" si="0"/>
         <v>1626.7889864947001</v>
       </c>
       <c r="H20" s="2" t="str">
-        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0041</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="11">
         <v>2.3430948519810001E-3</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="11">
         <v>0.27145285688584803</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="11">
         <v>4.1952614539950001E-2</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="11">
         <v>8.0329680558510006E-3</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="11">
         <v>1.0537654961971E-2</v>
       </c>
       <c r="G21" s="2">
-        <f>MAX(B21:F21)</f>
+        <f t="shared" si="0"/>
         <v>0.27145285688584803</v>
       </c>
       <c r="H21" s="2" t="str">
-        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="11">
         <v>4.4712238799999998E-7</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="11">
         <v>1.6256870339999999E-6</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="11">
         <v>3.3026496429450001E-3</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="11">
         <v>4.1844344166799998E-4</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="11">
         <v>1.0700632831299999E-4</v>
       </c>
       <c r="G22" s="2">
-        <f>MAX(B22:F22)</f>
+        <f t="shared" si="0"/>
         <v>3.3026496429450001E-3</v>
       </c>
       <c r="H22" s="2" t="str">
-        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="11">
         <v>2.9077729900000001E-7</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="11">
         <v>1.687767312E-6</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="11">
         <v>6.5404608780000001E-6</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="11">
         <v>8.0733784899999995E-7</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="11">
         <v>2.3141849456000001E-5</v>
       </c>
       <c r="G23" s="2">
-        <f>MAX(B23:F23)</f>
+        <f t="shared" si="0"/>
         <v>2.3141849456000001E-5</v>
       </c>
       <c r="H23" s="2" t="str">
-        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0044</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="11">
         <v>9.5372061717999995E-5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="11">
         <v>7.879318263E-6</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="11">
         <v>2.7857103249999999E-6</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="11">
         <v>1.114250656E-6</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="11">
         <v>1.6430287817E-5</v>
       </c>
       <c r="G24" s="2">
-        <f>MAX(B24:F24)</f>
+        <f t="shared" si="0"/>
         <v>9.5372061717999995E-5</v>
       </c>
       <c r="H24" s="2" t="str">
-        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="11">
         <v>8.9347272179800003E-4</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="11">
         <v>6.4164478208277004E-2</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="11">
         <v>1.4728892546029999E-3</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="11">
         <v>2.4748095038909998E-3</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="11">
         <v>3.6151556306640999E-2</v>
       </c>
       <c r="G25" s="2">
-        <f>MAX(B25:F25)</f>
+        <f t="shared" si="0"/>
         <v>6.4164478208277004E-2</v>
       </c>
       <c r="H25" s="2" t="str">
-        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="11">
         <v>1.3400424963200001E-4</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="11">
         <v>1.02900827827E-4</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="11">
         <v>7.4006982009000005E-5</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="11">
         <v>6.8290283139999997E-5</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="11">
         <v>2.988694298513E-3</v>
       </c>
       <c r="G26" s="2">
-        <f>MAX(B26:F26)</f>
+        <f t="shared" si="0"/>
         <v>2.988694298513E-3</v>
       </c>
       <c r="H26" s="2" t="str">
-        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0044</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="7">
+      <c r="I27" s="13">
         <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
         <v>0.52</v>
       </c>
@@ -4006,15 +4020,15 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
-        <f>MAX(B2:F2)</f>
+        <f t="shared" ref="G2:G26" si="0">MAX(B2:F2)</f>
         <v>0</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f>IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
+        <f t="shared" ref="H2:H26" si="1">IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
         <v>SV0001</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
+        <f t="shared" ref="I2:I26" si="2">IF(LEFT(A2,6)=H2, "Yes", "")</f>
         <v>Yes</v>
       </c>
     </row>
@@ -4028,15 +4042,15 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
-        <f>MAX(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H3" s="2" t="str">
-        <f>IF(G3=B3,$B$1,IF(G3=C3,$C$1,IF(G3=D3,$D$1,IF(G3=E3,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f>IF(LEFT(A3,6)=H3, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4050,15 +4064,15 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f>MAX(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" s="2" t="str">
-        <f>IF(G4=B4,$B$1,IF(G4=C4,$C$1,IF(G4=D4,$D$1,IF(G4=E4,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>IF(LEFT(A4,6)=H4, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4072,15 +4086,15 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <f>MAX(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" s="2" t="str">
-        <f>IF(G5=B5,$B$1,IF(G5=C5,$C$1,IF(G5=D5,$D$1,IF(G5=E5,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f>IF(LEFT(A5,6)=H5, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4094,15 +4108,15 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f>MAX(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="2" t="str">
-        <f>IF(G6=B6,$B$1,IF(G6=C6,$C$1,IF(G6=D6,$D$1,IF(G6=E6,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>IF(LEFT(A6,6)=H6, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4116,15 +4130,15 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f>MAX(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="2" t="str">
-        <f>IF(G7=B7,$B$1,IF(G7=C7,$C$1,IF(G7=D7,$D$1,IF(G7=E7,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I7" s="1" t="str">
-        <f>IF(LEFT(A7,6)=H7, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4138,15 +4152,15 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f>MAX(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="2" t="str">
-        <f>IF(G8=B8,$B$1,IF(G8=C8,$C$1,IF(G8=D8,$D$1,IF(G8=E8,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I8" s="1" t="str">
-        <f>IF(LEFT(A8,6)=H8, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4160,15 +4174,15 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f>MAX(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="2" t="str">
-        <f>IF(G9=B9,$B$1,IF(G9=C9,$C$1,IF(G9=D9,$D$1,IF(G9=E9,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I9" s="1" t="str">
-        <f>IF(LEFT(A9,6)=H9, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4182,15 +4196,15 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f>MAX(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="2" t="str">
-        <f>IF(G10=B10,$B$1,IF(G10=C10,$C$1,IF(G10=D10,$D$1,IF(G10=E10,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I10" s="1" t="str">
-        <f>IF(LEFT(A10,6)=H10, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4204,15 +4218,15 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f>MAX(B11:F11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="2" t="str">
-        <f>IF(G11=B11,$B$1,IF(G11=C11,$C$1,IF(G11=D11,$D$1,IF(G11=E11,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I11" s="1" t="str">
-        <f>IF(LEFT(A11,6)=H11, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4226,15 +4240,15 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <f>MAX(B12:F12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="2" t="str">
-        <f>IF(G12=B12,$B$1,IF(G12=C12,$C$1,IF(G12=D12,$D$1,IF(G12=E12,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I12" s="1" t="str">
-        <f>IF(LEFT(A12,6)=H12, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4248,15 +4262,15 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f>MAX(B13:F13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="2" t="str">
-        <f>IF(G13=B13,$B$1,IF(G13=C13,$C$1,IF(G13=D13,$D$1,IF(G13=E13,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I13" s="1" t="str">
-        <f>IF(LEFT(A13,6)=H13, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4270,15 +4284,15 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <f>MAX(B14:F14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="2" t="str">
-        <f>IF(G14=B14,$B$1,IF(G14=C14,$C$1,IF(G14=D14,$D$1,IF(G14=E14,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f>IF(LEFT(A14,6)=H14, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4292,15 +4306,15 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
-        <f>MAX(B15:F15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="2" t="str">
-        <f>IF(G15=B15,$B$1,IF(G15=C15,$C$1,IF(G15=D15,$D$1,IF(G15=E15,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I15" s="1" t="str">
-        <f>IF(LEFT(A15,6)=H15, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4314,15 +4328,15 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
-        <f>MAX(B16:F16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="2" t="str">
-        <f>IF(G16=B16,$B$1,IF(G16=C16,$C$1,IF(G16=D16,$D$1,IF(G16=E16,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I16" s="1" t="str">
-        <f>IF(LEFT(A16,6)=H16, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4336,15 +4350,15 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <f>MAX(B17:F17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="2" t="str">
-        <f>IF(G17=B17,$B$1,IF(G17=C17,$C$1,IF(G17=D17,$D$1,IF(G17=E17,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f>IF(LEFT(A17,6)=H17, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4358,15 +4372,15 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f>MAX(B18:F18)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="2" t="str">
-        <f>IF(G18=B18,$B$1,IF(G18=C18,$C$1,IF(G18=D18,$D$1,IF(G18=E18,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I18" s="1" t="str">
-        <f>IF(LEFT(A18,6)=H18, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4380,15 +4394,15 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f>MAX(B19:F19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="2" t="str">
-        <f>IF(G19=B19,$B$1,IF(G19=C19,$C$1,IF(G19=D19,$D$1,IF(G19=E19,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I19" s="1" t="str">
-        <f>IF(LEFT(A19,6)=H19, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4402,15 +4416,15 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f>MAX(B20:F20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="2" t="str">
-        <f>IF(G20=B20,$B$1,IF(G20=C20,$C$1,IF(G20=D20,$D$1,IF(G20=E20,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I20" s="1" t="str">
-        <f>IF(LEFT(A20,6)=H20, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4424,15 +4438,15 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f>MAX(B21:F21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="2" t="str">
-        <f>IF(G21=B21,$B$1,IF(G21=C21,$C$1,IF(G21=D21,$D$1,IF(G21=E21,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I21" s="1" t="str">
-        <f>IF(LEFT(A21,6)=H21, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4456,15 +4470,15 @@
         <v>8.9976757852999994E-5</v>
       </c>
       <c r="G22" s="2">
-        <f>MAX(B22:F22)</f>
+        <f t="shared" si="0"/>
         <v>2.4869391059069998E-3</v>
       </c>
       <c r="H22" s="2" t="str">
-        <f>IF(G22=B22,$B$1,IF(G22=C22,$C$1,IF(G22=D22,$D$1,IF(G22=E22,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0007</v>
       </c>
       <c r="I22" s="1" t="str">
-        <f>IF(LEFT(A22,6)=H22, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4488,15 +4502,15 @@
         <v>6.4386189484E-5</v>
       </c>
       <c r="G23" s="2">
-        <f>MAX(B23:F23)</f>
+        <f t="shared" si="0"/>
         <v>6.4386189484E-5</v>
       </c>
       <c r="H23" s="2" t="str">
-        <f>IF(G23=B23,$B$1,IF(G23=C23,$C$1,IF(G23=D23,$D$1,IF(G23=E23,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0044</v>
       </c>
       <c r="I23" s="1" t="str">
-        <f>IF(LEFT(A23,6)=H23, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>
@@ -4520,15 +4534,15 @@
         <v>3.2852448390999999E-5</v>
       </c>
       <c r="G24" s="2">
-        <f>MAX(B24:F24)</f>
+        <f t="shared" si="0"/>
         <v>9.4832263917000005E-5</v>
       </c>
       <c r="H24" s="2" t="str">
-        <f>IF(G24=B24,$B$1,IF(G24=C24,$C$1,IF(G24=D24,$D$1,IF(G24=E24,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0001</v>
       </c>
       <c r="I24" s="1" t="str">
-        <f>IF(LEFT(A24,6)=H24, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4552,15 +4566,15 @@
         <v>8.4026184479928004E-2</v>
       </c>
       <c r="G25" s="2">
-        <f>MAX(B25:F25)</f>
+        <f t="shared" si="0"/>
         <v>0.12783303428942799</v>
       </c>
       <c r="H25" s="2" t="str">
-        <f>IF(G25=B25,$B$1,IF(G25=C25,$C$1,IF(G25=D25,$D$1,IF(G25=E25,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0002</v>
       </c>
       <c r="I25" s="1" t="str">
-        <f>IF(LEFT(A25,6)=H25, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -4584,15 +4598,15 @@
         <v>4.2195553201679996E-3</v>
       </c>
       <c r="G26" s="2">
-        <f>MAX(B26:F26)</f>
+        <f t="shared" si="0"/>
         <v>4.2195553201679996E-3</v>
       </c>
       <c r="H26" s="2" t="str">
-        <f>IF(G26=B26,$B$1,IF(G26=C26,$C$1,IF(G26=D26,$D$1,IF(G26=E26,$E$1,$F$1))))</f>
+        <f t="shared" si="1"/>
         <v>SV0044</v>
       </c>
       <c r="I26" s="1" t="str">
-        <f>IF(LEFT(A26,6)=H26, "Yes", "")</f>
+        <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lab1 - Bổ sung bộ train1/test1 (đã cắt silence). - Bổ sung thống kê kết quả.
</commit_message>
<xml_diff>
--- a/Lab1/Statistic.xlsx
+++ b/Lab1/Statistic.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Gauss_1" sheetId="1" r:id="rId1"/>
     <sheet name="Gauss_2" sheetId="3" r:id="rId2"/>
     <sheet name="GMM_1" sheetId="2" r:id="rId3"/>
     <sheet name="GMM_2" sheetId="4" r:id="rId4"/>
-    <sheet name="GMM_3" sheetId="5" r:id="rId5"/>
+    <sheet name="General" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="54">
   <si>
     <t>SV0001_23</t>
   </si>
@@ -143,19 +143,56 @@
     <t>(25,100)</t>
   </si>
   <si>
-    <t>(38,100)</t>
+    <t>Result (cut)</t>
+  </si>
+  <si>
+    <t>(5,100)</t>
+  </si>
+  <si>
+    <t>(10,100)</t>
+  </si>
+  <si>
+    <t>Acc</t>
+  </si>
+  <si>
+    <t>(7,100)</t>
+  </si>
+  <si>
+    <t>(2,100)</t>
+  </si>
+  <si>
+    <t>(4,100)</t>
+  </si>
+  <si>
+    <t>(6,100)</t>
+  </si>
+  <si>
+    <t>(37,100)</t>
+  </si>
+  <si>
+    <t>(5,50)</t>
+  </si>
+  <si>
+    <t>(5,150)</t>
+  </si>
+  <si>
+    <t>(5,25)</t>
+  </si>
+  <si>
+    <t>(5,37)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000000"/>
-    <numFmt numFmtId="180" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +203,42 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -229,16 +302,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,9 +1491,10 @@
     <col min="2" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>25</v>
@@ -1437,8 +1520,14 @@
       <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1469,8 +1558,15 @@
         <f>IF(LEFT(A2,6)=H2, "Yes", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>IF(LEFT(A2,6)=J2, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1501,8 +1597,15 @@
         <f t="shared" ref="I3:I26" si="2">IF(LEFT(A3,6)=H3, "Yes", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:K26" si="3">IF(LEFT(A3,6)=J3, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1533,8 +1636,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1565,8 +1675,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1597,8 +1714,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1629,8 +1753,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1661,8 +1792,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1693,8 +1831,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1725,8 +1870,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1757,8 +1909,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1789,8 +1948,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1821,8 +1987,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1853,8 +2026,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1885,8 +2065,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1917,8 +2104,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1949,8 +2143,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1981,8 +2182,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -2013,8 +2221,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2045,8 +2260,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -2077,8 +2299,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -2109,8 +2338,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -2141,8 +2377,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
@@ -2173,8 +2416,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
@@ -2205,8 +2455,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
@@ -2237,15 +2494,27 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I27" s="7">
         <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
         <v>0.28000000000000003</v>
       </c>
+      <c r="K27" s="7">
+        <f t="shared" ref="K27" si="4">COUNTIF(K2:K26,"Yes")/COUNTA(K2:K26)</f>
+        <v>0.8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3107,9 +3376,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3121,9 +3390,10 @@
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>40</v>
       </c>
@@ -3151,8 +3421,14 @@
       <c r="I1" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -3183,8 +3459,15 @@
         <f t="shared" ref="I2:I26" si="2">IF(LEFT(A2,6)=H2, "Yes", "")</f>
         <v/>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="str">
+        <f>IF(LEFT(A2,6)=J2, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
@@ -3215,8 +3498,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" ref="K3:K26" si="3">IF(LEFT(A3,6)=J3, "Yes", "")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
@@ -3247,8 +3537,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -3279,8 +3576,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -3311,8 +3615,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -3343,8 +3654,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -3375,8 +3693,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
@@ -3407,8 +3732,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -3439,8 +3771,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>9</v>
       </c>
@@ -3471,8 +3810,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>10</v>
       </c>
@@ -3503,8 +3849,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -3535,8 +3888,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>12</v>
       </c>
@@ -3567,8 +3927,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
@@ -3599,8 +3966,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -3631,8 +4005,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>20</v>
       </c>
@@ -3663,8 +4044,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>21</v>
       </c>
@@ -3695,8 +4083,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>22</v>
       </c>
@@ -3727,8 +4122,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>23</v>
       </c>
@@ -3759,8 +4161,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>24</v>
       </c>
@@ -3791,8 +4200,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>35</v>
       </c>
@@ -3823,8 +4239,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>36</v>
       </c>
@@ -3855,8 +4278,15 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
@@ -3887,8 +4317,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>38</v>
       </c>
@@ -3919,8 +4356,15 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>39</v>
       </c>
@@ -3951,11 +4395,22 @@
         <f t="shared" si="2"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I27" s="13">
         <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
         <v>0.52</v>
+      </c>
+      <c r="K27" s="13">
+        <f>COUNTIF(K2:K26,"Yes")/COUNTA(K2:K26)</f>
+        <v>0.72</v>
       </c>
     </row>
   </sheetData>
@@ -3965,658 +4420,879 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
-        <f t="shared" ref="G2:G26" si="0">MAX(B2:F2)</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f t="shared" ref="H2:H26" si="1">IF(G2=B2,$B$1,IF(G2=C2,$C$1,IF(G2=D2,$D$1,IF(G2=E2,$E$1,$F$1))))</f>
-        <v>SV0001</v>
-      </c>
-      <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:I26" si="2">IF(LEFT(A2,6)=H2, "Yes", "")</f>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I3" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="2">
-        <v>3.43365188E-7</v>
-      </c>
-      <c r="C22" s="2">
-        <v>1.468321426E-6</v>
-      </c>
-      <c r="D22" s="2">
-        <v>2.4869391059069998E-3</v>
-      </c>
-      <c r="E22" s="2">
-        <v>8.1619302808999994E-5</v>
-      </c>
-      <c r="F22" s="2">
-        <v>8.9976757852999994E-5</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>2.4869391059069998E-3</v>
-      </c>
-      <c r="H22" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0007</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="2">
-        <v>4.1233670800000002E-7</v>
-      </c>
-      <c r="C23" s="2">
-        <v>1.100811068E-6</v>
-      </c>
-      <c r="D23" s="2">
-        <v>6.2640250230000003E-6</v>
-      </c>
-      <c r="E23" s="2">
-        <v>3.2215572520000001E-6</v>
-      </c>
-      <c r="F23" s="2">
-        <v>6.4386189484E-5</v>
-      </c>
-      <c r="G23" s="2">
-        <f t="shared" si="0"/>
-        <v>6.4386189484E-5</v>
-      </c>
-      <c r="H23" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0044</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2">
-        <v>9.4832263917000005E-5</v>
-      </c>
-      <c r="C24" s="2">
-        <v>5.3023832559999997E-6</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1.880532427E-6</v>
-      </c>
-      <c r="E24" s="2">
-        <v>2.0470341900000002E-6</v>
-      </c>
-      <c r="F24" s="2">
-        <v>3.2852448390999999E-5</v>
-      </c>
-      <c r="G24" s="2">
-        <f t="shared" si="0"/>
-        <v>9.4832263917000005E-5</v>
-      </c>
-      <c r="H24" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0001</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="2">
-        <v>7.9485853244999996E-4</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.12783303428942799</v>
-      </c>
-      <c r="D25" s="2">
-        <v>9.2142152476160002E-3</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2.2619171550639998E-3</v>
-      </c>
-      <c r="F25" s="2">
-        <v>8.4026184479928004E-2</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.12783303428942799</v>
-      </c>
-      <c r="H25" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0002</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="M25" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="2">
-        <v>1.6935860305299999E-4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>4.8501551259999998E-5</v>
-      </c>
-      <c r="D26" s="2">
-        <v>1.01855893874E-4</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1.6114369497799999E-4</v>
-      </c>
-      <c r="F26" s="2">
-        <v>4.2195553201679996E-3</v>
-      </c>
-      <c r="G26" s="2">
-        <f t="shared" si="0"/>
-        <v>4.2195553201679996E-3</v>
-      </c>
-      <c r="H26" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>SV0044</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Yes</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="7">
-        <f>COUNTIF(I2:I26,"Yes")/COUNTA(I2:I26)</f>
-        <v>0.28000000000000003</v>
-      </c>
+      <c r="B26" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="22">
+        <f>(25-2)/25</f>
+        <v>0.92</v>
+      </c>
+      <c r="F27" s="21">
+        <f>(25-1)/25</f>
+        <v>0.96</v>
+      </c>
+      <c r="G27" s="22">
+        <f>(25-2)/25</f>
+        <v>0.92</v>
+      </c>
+      <c r="H27" s="21"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="19">
+        <f>(25-7)/25</f>
+        <v>0.72</v>
+      </c>
+      <c r="L27" s="19">
+        <f>(25-7)/25</f>
+        <v>0.72</v>
+      </c>
+      <c r="M27" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F27" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>